<commit_message>
changes to model 7/3/2018
</commit_message>
<xml_diff>
--- a/4-25 model/AMR_Datasheet.xlsx
+++ b/4-25 model/AMR_Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Yale\CIDMA\AMR\Carbapenem-Resistance\4-25 model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C59788AA-F871-4B64-A4A9-3AA489F0628C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F0CF9D-0194-4DB7-9438-E24F2885B603}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="2180" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="2180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pneu_model" sheetId="13" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Resistance (CDDEP + Merck)" sheetId="18" r:id="rId8"/>
     <sheet name="R freq. (CDDEP + Merck)" sheetId="19" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="212">
   <si>
     <t>Year</t>
   </si>
@@ -1870,6 +1870,12 @@
   <si>
     <t>cIAI attributed to KP</t>
   </si>
+  <si>
+    <t>Proportion of pneumonia patients prescribed CBP</t>
+  </si>
+  <si>
+    <t>Pneumonia prescribed CBP (Merck)</t>
+  </si>
 </sst>
 </file>
 
@@ -2210,7 +2216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2369,6 +2375,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2384,13 +2397,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2671,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3138,49 +3154,49 @@
       <c r="A10" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="97">
+      <c r="B10" s="92">
         <v>0</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="92">
         <v>1</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="92">
         <v>4</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="92">
         <v>3</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="92">
         <v>2</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="92">
         <v>0</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H10" s="92">
         <v>2</v>
       </c>
-      <c r="I10" s="97">
+      <c r="I10" s="92">
         <v>0</v>
       </c>
-      <c r="J10" s="97">
+      <c r="J10" s="92">
         <v>0</v>
       </c>
-      <c r="K10" s="97">
+      <c r="K10" s="92">
         <v>5</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="92">
         <v>4</v>
       </c>
-      <c r="M10" s="97">
+      <c r="M10" s="92">
         <v>9</v>
       </c>
-      <c r="N10" s="97">
+      <c r="N10" s="92">
         <v>3</v>
       </c>
-      <c r="O10" s="97">
+      <c r="O10" s="92">
         <v>6</v>
       </c>
-      <c r="P10" s="97">
+      <c r="P10" s="92">
         <v>8</v>
       </c>
       <c r="Q10" s="19"/>
@@ -3191,49 +3207,49 @@
       <c r="A11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="92">
         <v>0</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="92">
         <v>0</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="92">
         <v>0</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="92">
         <v>1</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="92">
         <v>2</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="92">
         <v>0</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="92">
         <v>1</v>
       </c>
-      <c r="I11" s="97">
+      <c r="I11" s="92">
         <v>0</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J11" s="92">
         <v>0</v>
       </c>
-      <c r="K11" s="97">
+      <c r="K11" s="92">
         <v>1</v>
       </c>
-      <c r="L11" s="97">
+      <c r="L11" s="92">
         <v>0</v>
       </c>
-      <c r="M11" s="97">
+      <c r="M11" s="92">
         <v>0</v>
       </c>
-      <c r="N11" s="97">
+      <c r="N11" s="92">
         <v>1</v>
       </c>
-      <c r="O11" s="97">
+      <c r="O11" s="92">
         <v>0</v>
       </c>
-      <c r="P11" s="97">
+      <c r="P11" s="92">
         <v>0</v>
       </c>
       <c r="Q11" s="19"/>
@@ -3835,7 +3851,7 @@
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A33" s="76" t="s">
         <v>117</v>
       </c>
@@ -3885,7 +3901,7 @@
         <v>1012690.3223150712</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A34" s="77" t="s">
         <v>191</v>
       </c>
@@ -3913,7 +3929,7 @@
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A35" s="88" t="s">
         <v>192</v>
       </c>
@@ -3942,7 +3958,7 @@
       <c r="O35" s="32"/>
       <c r="P35" s="32"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A36" s="88" t="s">
         <v>193</v>
       </c>
@@ -3969,7 +3985,7 @@
       <c r="O36" s="32"/>
       <c r="P36" s="32"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A37" s="88" t="s">
         <v>195</v>
       </c>
@@ -3999,7 +4015,7 @@
       <c r="O37" s="32"/>
       <c r="P37" s="32"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A38" s="88" t="s">
         <v>201</v>
       </c>
@@ -4028,7 +4044,7 @@
       <c r="O38" s="32"/>
       <c r="P38" s="32"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A39" s="88" t="s">
         <v>196</v>
       </c>
@@ -4056,7 +4072,7 @@
       <c r="O39" s="32"/>
       <c r="P39" s="32"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A40" s="88" t="s">
         <v>197</v>
       </c>
@@ -4084,7 +4100,7 @@
       <c r="O40" s="32"/>
       <c r="P40" s="32"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A41" s="88" t="s">
         <v>198</v>
       </c>
@@ -4112,7 +4128,7 @@
       <c r="O41" s="32"/>
       <c r="P41" s="32"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="A42" s="88" t="s">
         <v>199</v>
       </c>
@@ -4140,24 +4156,1066 @@
       <c r="O42" s="32"/>
       <c r="P42" s="32"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B43" s="32"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
+    <row r="43" spans="1:1025" s="104" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="105" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43" s="32">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="C43" s="32">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D43" s="32">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="E43" s="32">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="F43" s="32">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="G43" s="32">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="H43" s="32">
+        <v>1.12E-2</v>
+      </c>
+      <c r="I43" s="32">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="J43" s="32">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="K43" s="32">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="L43" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="M43" s="32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N43" s="32">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="O43" s="32">
+        <v>6.6E-3</v>
+      </c>
+      <c r="P43" s="32">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="102"/>
+      <c r="T43" s="103"/>
+      <c r="U43" s="103"/>
+      <c r="V43" s="103"/>
+      <c r="W43" s="103"/>
+      <c r="X43" s="103"/>
+      <c r="Y43" s="103"/>
+      <c r="Z43" s="103"/>
+      <c r="AA43" s="103"/>
+      <c r="AB43" s="103"/>
+      <c r="AC43" s="103"/>
+      <c r="AD43" s="103"/>
+      <c r="AE43" s="103"/>
+      <c r="AF43" s="103"/>
+      <c r="AG43" s="103"/>
+      <c r="AH43" s="103"/>
+      <c r="AI43" s="103"/>
+      <c r="AJ43" s="103"/>
+      <c r="AK43" s="103"/>
+      <c r="AL43" s="103"/>
+      <c r="AM43" s="103"/>
+      <c r="AN43" s="103"/>
+      <c r="AO43" s="103"/>
+      <c r="AP43" s="103"/>
+      <c r="AQ43" s="103"/>
+      <c r="AR43" s="103"/>
+      <c r="AS43" s="103"/>
+      <c r="AT43" s="103"/>
+      <c r="AU43" s="103"/>
+      <c r="AV43" s="103"/>
+      <c r="AW43" s="103"/>
+      <c r="AX43" s="103"/>
+      <c r="AY43" s="103"/>
+      <c r="AZ43" s="103"/>
+      <c r="BA43" s="103"/>
+      <c r="BB43" s="103"/>
+      <c r="BC43" s="103"/>
+      <c r="BD43" s="103"/>
+      <c r="BE43" s="103"/>
+      <c r="BF43" s="103"/>
+      <c r="BG43" s="103"/>
+      <c r="BH43" s="103"/>
+      <c r="BI43" s="103"/>
+      <c r="BJ43" s="103"/>
+      <c r="BK43" s="103"/>
+      <c r="BL43" s="103"/>
+      <c r="BM43" s="103"/>
+      <c r="BN43" s="103"/>
+      <c r="BO43" s="103"/>
+      <c r="BP43" s="103"/>
+      <c r="BQ43" s="103"/>
+      <c r="BR43" s="103"/>
+      <c r="BS43" s="103"/>
+      <c r="BT43" s="103"/>
+      <c r="BU43" s="103"/>
+      <c r="BV43" s="103"/>
+      <c r="BW43" s="103"/>
+      <c r="BX43" s="103"/>
+      <c r="BY43" s="103"/>
+      <c r="BZ43" s="103"/>
+      <c r="CA43" s="103"/>
+      <c r="CB43" s="103"/>
+      <c r="CC43" s="103"/>
+      <c r="CD43" s="103"/>
+      <c r="CE43" s="103"/>
+      <c r="CF43" s="103"/>
+      <c r="CG43" s="103"/>
+      <c r="CH43" s="103"/>
+      <c r="CI43" s="103"/>
+      <c r="CJ43" s="103"/>
+      <c r="CK43" s="103"/>
+      <c r="CL43" s="103"/>
+      <c r="CM43" s="103"/>
+      <c r="CN43" s="103"/>
+      <c r="CO43" s="103"/>
+      <c r="CP43" s="103"/>
+      <c r="CQ43" s="103"/>
+      <c r="CR43" s="103"/>
+      <c r="CS43" s="103"/>
+      <c r="CT43" s="103"/>
+      <c r="CU43" s="103"/>
+      <c r="CV43" s="103"/>
+      <c r="CW43" s="103"/>
+      <c r="CX43" s="103"/>
+      <c r="CY43" s="103"/>
+      <c r="CZ43" s="103"/>
+      <c r="DA43" s="103"/>
+      <c r="DB43" s="103"/>
+      <c r="DC43" s="103"/>
+      <c r="DD43" s="103"/>
+      <c r="DE43" s="103"/>
+      <c r="DF43" s="103"/>
+      <c r="DG43" s="103"/>
+      <c r="DH43" s="103"/>
+      <c r="DI43" s="103"/>
+      <c r="DJ43" s="103"/>
+      <c r="DK43" s="103"/>
+      <c r="DL43" s="103"/>
+      <c r="DM43" s="103"/>
+      <c r="DN43" s="103"/>
+      <c r="DO43" s="103"/>
+      <c r="DP43" s="103"/>
+      <c r="DQ43" s="103"/>
+      <c r="DR43" s="103"/>
+      <c r="DS43" s="103"/>
+      <c r="DT43" s="103"/>
+      <c r="DU43" s="103"/>
+      <c r="DV43" s="103"/>
+      <c r="DW43" s="103"/>
+      <c r="DX43" s="103"/>
+      <c r="DY43" s="103"/>
+      <c r="DZ43" s="103"/>
+      <c r="EA43" s="103"/>
+      <c r="EB43" s="103"/>
+      <c r="EC43" s="103"/>
+      <c r="ED43" s="103"/>
+      <c r="EE43" s="103"/>
+      <c r="EF43" s="103"/>
+      <c r="EG43" s="103"/>
+      <c r="EH43" s="103"/>
+      <c r="EI43" s="103"/>
+      <c r="EJ43" s="103"/>
+      <c r="EK43" s="103"/>
+      <c r="EL43" s="103"/>
+      <c r="EM43" s="103"/>
+      <c r="EN43" s="103"/>
+      <c r="EO43" s="103"/>
+      <c r="EP43" s="103"/>
+      <c r="EQ43" s="103"/>
+      <c r="ER43" s="103"/>
+      <c r="ES43" s="103"/>
+      <c r="ET43" s="103"/>
+      <c r="EU43" s="103"/>
+      <c r="EV43" s="103"/>
+      <c r="EW43" s="103"/>
+      <c r="EX43" s="103"/>
+      <c r="EY43" s="103"/>
+      <c r="EZ43" s="103"/>
+      <c r="FA43" s="103"/>
+      <c r="FB43" s="103"/>
+      <c r="FC43" s="103"/>
+      <c r="FD43" s="103"/>
+      <c r="FE43" s="103"/>
+      <c r="FF43" s="103"/>
+      <c r="FG43" s="103"/>
+      <c r="FH43" s="103"/>
+      <c r="FI43" s="103"/>
+      <c r="FJ43" s="103"/>
+      <c r="FK43" s="103"/>
+      <c r="FL43" s="103"/>
+      <c r="FM43" s="103"/>
+      <c r="FN43" s="103"/>
+      <c r="FO43" s="103"/>
+      <c r="FP43" s="103"/>
+      <c r="FQ43" s="103"/>
+      <c r="FR43" s="103"/>
+      <c r="FS43" s="103"/>
+      <c r="FT43" s="103"/>
+      <c r="FU43" s="103"/>
+      <c r="FV43" s="103"/>
+      <c r="FW43" s="103"/>
+      <c r="FX43" s="103"/>
+      <c r="FY43" s="103"/>
+      <c r="FZ43" s="103"/>
+      <c r="GA43" s="103"/>
+      <c r="GB43" s="103"/>
+      <c r="GC43" s="103"/>
+      <c r="GD43" s="103"/>
+      <c r="GE43" s="103"/>
+      <c r="GF43" s="103"/>
+      <c r="GG43" s="103"/>
+      <c r="GH43" s="103"/>
+      <c r="GI43" s="103"/>
+      <c r="GJ43" s="103"/>
+      <c r="GK43" s="103"/>
+      <c r="GL43" s="103"/>
+      <c r="GM43" s="103"/>
+      <c r="GN43" s="103"/>
+      <c r="GO43" s="103"/>
+      <c r="GP43" s="103"/>
+      <c r="GQ43" s="103"/>
+      <c r="GR43" s="103"/>
+      <c r="GS43" s="103"/>
+      <c r="GT43" s="103"/>
+      <c r="GU43" s="103"/>
+      <c r="GV43" s="103"/>
+      <c r="GW43" s="103"/>
+      <c r="GX43" s="103"/>
+      <c r="GY43" s="103"/>
+      <c r="GZ43" s="103"/>
+      <c r="HA43" s="103"/>
+      <c r="HB43" s="103"/>
+      <c r="HC43" s="103"/>
+      <c r="HD43" s="103"/>
+      <c r="HE43" s="103"/>
+      <c r="HF43" s="103"/>
+      <c r="HG43" s="103"/>
+      <c r="HH43" s="103"/>
+      <c r="HI43" s="103"/>
+      <c r="HJ43" s="103"/>
+      <c r="HK43" s="103"/>
+      <c r="HL43" s="103"/>
+      <c r="HM43" s="103"/>
+      <c r="HN43" s="103"/>
+      <c r="HO43" s="103"/>
+      <c r="HP43" s="103"/>
+      <c r="HQ43" s="103"/>
+      <c r="HR43" s="103"/>
+      <c r="HS43" s="103"/>
+      <c r="HT43" s="103"/>
+      <c r="HU43" s="103"/>
+      <c r="HV43" s="103"/>
+      <c r="HW43" s="103"/>
+      <c r="HX43" s="103"/>
+      <c r="HY43" s="103"/>
+      <c r="HZ43" s="103"/>
+      <c r="IA43" s="103"/>
+      <c r="IB43" s="103"/>
+      <c r="IC43" s="103"/>
+      <c r="ID43" s="103"/>
+      <c r="IE43" s="103"/>
+      <c r="IF43" s="103"/>
+      <c r="IG43" s="103"/>
+      <c r="IH43" s="103"/>
+      <c r="II43" s="103"/>
+      <c r="IJ43" s="103"/>
+      <c r="IK43" s="103"/>
+      <c r="IL43" s="103"/>
+      <c r="IM43" s="103"/>
+      <c r="IN43" s="103"/>
+      <c r="IO43" s="103"/>
+      <c r="IP43" s="103"/>
+      <c r="IQ43" s="103"/>
+      <c r="IR43" s="103"/>
+      <c r="IS43" s="103"/>
+      <c r="IT43" s="103"/>
+      <c r="IU43" s="103"/>
+      <c r="IV43" s="103"/>
+      <c r="IW43" s="103"/>
+      <c r="IX43" s="103"/>
+      <c r="IY43" s="103"/>
+      <c r="IZ43" s="103"/>
+      <c r="JA43" s="103"/>
+      <c r="JB43" s="103"/>
+      <c r="JC43" s="103"/>
+      <c r="JD43" s="103"/>
+      <c r="JE43" s="103"/>
+      <c r="JF43" s="103"/>
+      <c r="JG43" s="103"/>
+      <c r="JH43" s="103"/>
+      <c r="JI43" s="103"/>
+      <c r="JJ43" s="103"/>
+      <c r="JK43" s="103"/>
+      <c r="JL43" s="103"/>
+      <c r="JM43" s="103"/>
+      <c r="JN43" s="103"/>
+      <c r="JO43" s="103"/>
+      <c r="JP43" s="103"/>
+      <c r="JQ43" s="103"/>
+      <c r="JR43" s="103"/>
+      <c r="JS43" s="103"/>
+      <c r="JT43" s="103"/>
+      <c r="JU43" s="103"/>
+      <c r="JV43" s="103"/>
+      <c r="JW43" s="103"/>
+      <c r="JX43" s="103"/>
+      <c r="JY43" s="103"/>
+      <c r="JZ43" s="103"/>
+      <c r="KA43" s="103"/>
+      <c r="KB43" s="103"/>
+      <c r="KC43" s="103"/>
+      <c r="KD43" s="103"/>
+      <c r="KE43" s="103"/>
+      <c r="KF43" s="103"/>
+      <c r="KG43" s="103"/>
+      <c r="KH43" s="103"/>
+      <c r="KI43" s="103"/>
+      <c r="KJ43" s="103"/>
+      <c r="KK43" s="103"/>
+      <c r="KL43" s="103"/>
+      <c r="KM43" s="103"/>
+      <c r="KN43" s="103"/>
+      <c r="KO43" s="103"/>
+      <c r="KP43" s="103"/>
+      <c r="KQ43" s="103"/>
+      <c r="KR43" s="103"/>
+      <c r="KS43" s="103"/>
+      <c r="KT43" s="103"/>
+      <c r="KU43" s="103"/>
+      <c r="KV43" s="103"/>
+      <c r="KW43" s="103"/>
+      <c r="KX43" s="103"/>
+      <c r="KY43" s="103"/>
+      <c r="KZ43" s="103"/>
+      <c r="LA43" s="103"/>
+      <c r="LB43" s="103"/>
+      <c r="LC43" s="103"/>
+      <c r="LD43" s="103"/>
+      <c r="LE43" s="103"/>
+      <c r="LF43" s="103"/>
+      <c r="LG43" s="103"/>
+      <c r="LH43" s="103"/>
+      <c r="LI43" s="103"/>
+      <c r="LJ43" s="103"/>
+      <c r="LK43" s="103"/>
+      <c r="LL43" s="103"/>
+      <c r="LM43" s="103"/>
+      <c r="LN43" s="103"/>
+      <c r="LO43" s="103"/>
+      <c r="LP43" s="103"/>
+      <c r="LQ43" s="103"/>
+      <c r="LR43" s="103"/>
+      <c r="LS43" s="103"/>
+      <c r="LT43" s="103"/>
+      <c r="LU43" s="103"/>
+      <c r="LV43" s="103"/>
+      <c r="LW43" s="103"/>
+      <c r="LX43" s="103"/>
+      <c r="LY43" s="103"/>
+      <c r="LZ43" s="103"/>
+      <c r="MA43" s="103"/>
+      <c r="MB43" s="103"/>
+      <c r="MC43" s="103"/>
+      <c r="MD43" s="103"/>
+      <c r="ME43" s="103"/>
+      <c r="MF43" s="103"/>
+      <c r="MG43" s="103"/>
+      <c r="MH43" s="103"/>
+      <c r="MI43" s="103"/>
+      <c r="MJ43" s="103"/>
+      <c r="MK43" s="103"/>
+      <c r="ML43" s="103"/>
+      <c r="MM43" s="103"/>
+      <c r="MN43" s="103"/>
+      <c r="MO43" s="103"/>
+      <c r="MP43" s="103"/>
+      <c r="MQ43" s="103"/>
+      <c r="MR43" s="103"/>
+      <c r="MS43" s="103"/>
+      <c r="MT43" s="103"/>
+      <c r="MU43" s="103"/>
+      <c r="MV43" s="103"/>
+      <c r="MW43" s="103"/>
+      <c r="MX43" s="103"/>
+      <c r="MY43" s="103"/>
+      <c r="MZ43" s="103"/>
+      <c r="NA43" s="103"/>
+      <c r="NB43" s="103"/>
+      <c r="NC43" s="103"/>
+      <c r="ND43" s="103"/>
+      <c r="NE43" s="103"/>
+      <c r="NF43" s="103"/>
+      <c r="NG43" s="103"/>
+      <c r="NH43" s="103"/>
+      <c r="NI43" s="103"/>
+      <c r="NJ43" s="103"/>
+      <c r="NK43" s="103"/>
+      <c r="NL43" s="103"/>
+      <c r="NM43" s="103"/>
+      <c r="NN43" s="103"/>
+      <c r="NO43" s="103"/>
+      <c r="NP43" s="103"/>
+      <c r="NQ43" s="103"/>
+      <c r="NR43" s="103"/>
+      <c r="NS43" s="103"/>
+      <c r="NT43" s="103"/>
+      <c r="NU43" s="103"/>
+      <c r="NV43" s="103"/>
+      <c r="NW43" s="103"/>
+      <c r="NX43" s="103"/>
+      <c r="NY43" s="103"/>
+      <c r="NZ43" s="103"/>
+      <c r="OA43" s="103"/>
+      <c r="OB43" s="103"/>
+      <c r="OC43" s="103"/>
+      <c r="OD43" s="103"/>
+      <c r="OE43" s="103"/>
+      <c r="OF43" s="103"/>
+      <c r="OG43" s="103"/>
+      <c r="OH43" s="103"/>
+      <c r="OI43" s="103"/>
+      <c r="OJ43" s="103"/>
+      <c r="OK43" s="103"/>
+      <c r="OL43" s="103"/>
+      <c r="OM43" s="103"/>
+      <c r="ON43" s="103"/>
+      <c r="OO43" s="103"/>
+      <c r="OP43" s="103"/>
+      <c r="OQ43" s="103"/>
+      <c r="OR43" s="103"/>
+      <c r="OS43" s="103"/>
+      <c r="OT43" s="103"/>
+      <c r="OU43" s="103"/>
+      <c r="OV43" s="103"/>
+      <c r="OW43" s="103"/>
+      <c r="OX43" s="103"/>
+      <c r="OY43" s="103"/>
+      <c r="OZ43" s="103"/>
+      <c r="PA43" s="103"/>
+      <c r="PB43" s="103"/>
+      <c r="PC43" s="103"/>
+      <c r="PD43" s="103"/>
+      <c r="PE43" s="103"/>
+      <c r="PF43" s="103"/>
+      <c r="PG43" s="103"/>
+      <c r="PH43" s="103"/>
+      <c r="PI43" s="103"/>
+      <c r="PJ43" s="103"/>
+      <c r="PK43" s="103"/>
+      <c r="PL43" s="103"/>
+      <c r="PM43" s="103"/>
+      <c r="PN43" s="103"/>
+      <c r="PO43" s="103"/>
+      <c r="PP43" s="103"/>
+      <c r="PQ43" s="103"/>
+      <c r="PR43" s="103"/>
+      <c r="PS43" s="103"/>
+      <c r="PT43" s="103"/>
+      <c r="PU43" s="103"/>
+      <c r="PV43" s="103"/>
+      <c r="PW43" s="103"/>
+      <c r="PX43" s="103"/>
+      <c r="PY43" s="103"/>
+      <c r="PZ43" s="103"/>
+      <c r="QA43" s="103"/>
+      <c r="QB43" s="103"/>
+      <c r="QC43" s="103"/>
+      <c r="QD43" s="103"/>
+      <c r="QE43" s="103"/>
+      <c r="QF43" s="103"/>
+      <c r="QG43" s="103"/>
+      <c r="QH43" s="103"/>
+      <c r="QI43" s="103"/>
+      <c r="QJ43" s="103"/>
+      <c r="QK43" s="103"/>
+      <c r="QL43" s="103"/>
+      <c r="QM43" s="103"/>
+      <c r="QN43" s="103"/>
+      <c r="QO43" s="103"/>
+      <c r="QP43" s="103"/>
+      <c r="QQ43" s="103"/>
+      <c r="QR43" s="103"/>
+      <c r="QS43" s="103"/>
+      <c r="QT43" s="103"/>
+      <c r="QU43" s="103"/>
+      <c r="QV43" s="103"/>
+      <c r="QW43" s="103"/>
+      <c r="QX43" s="103"/>
+      <c r="QY43" s="103"/>
+      <c r="QZ43" s="103"/>
+      <c r="RA43" s="103"/>
+      <c r="RB43" s="103"/>
+      <c r="RC43" s="103"/>
+      <c r="RD43" s="103"/>
+      <c r="RE43" s="103"/>
+      <c r="RF43" s="103"/>
+      <c r="RG43" s="103"/>
+      <c r="RH43" s="103"/>
+      <c r="RI43" s="103"/>
+      <c r="RJ43" s="103"/>
+      <c r="RK43" s="103"/>
+      <c r="RL43" s="103"/>
+      <c r="RM43" s="103"/>
+      <c r="RN43" s="103"/>
+      <c r="RO43" s="103"/>
+      <c r="RP43" s="103"/>
+      <c r="RQ43" s="103"/>
+      <c r="RR43" s="103"/>
+      <c r="RS43" s="103"/>
+      <c r="RT43" s="103"/>
+      <c r="RU43" s="103"/>
+      <c r="RV43" s="103"/>
+      <c r="RW43" s="103"/>
+      <c r="RX43" s="103"/>
+      <c r="RY43" s="103"/>
+      <c r="RZ43" s="103"/>
+      <c r="SA43" s="103"/>
+      <c r="SB43" s="103"/>
+      <c r="SC43" s="103"/>
+      <c r="SD43" s="103"/>
+      <c r="SE43" s="103"/>
+      <c r="SF43" s="103"/>
+      <c r="SG43" s="103"/>
+      <c r="SH43" s="103"/>
+      <c r="SI43" s="103"/>
+      <c r="SJ43" s="103"/>
+      <c r="SK43" s="103"/>
+      <c r="SL43" s="103"/>
+      <c r="SM43" s="103"/>
+      <c r="SN43" s="103"/>
+      <c r="SO43" s="103"/>
+      <c r="SP43" s="103"/>
+      <c r="SQ43" s="103"/>
+      <c r="SR43" s="103"/>
+      <c r="SS43" s="103"/>
+      <c r="ST43" s="103"/>
+      <c r="SU43" s="103"/>
+      <c r="SV43" s="103"/>
+      <c r="SW43" s="103"/>
+      <c r="SX43" s="103"/>
+      <c r="SY43" s="103"/>
+      <c r="SZ43" s="103"/>
+      <c r="TA43" s="103"/>
+      <c r="TB43" s="103"/>
+      <c r="TC43" s="103"/>
+      <c r="TD43" s="103"/>
+      <c r="TE43" s="103"/>
+      <c r="TF43" s="103"/>
+      <c r="TG43" s="103"/>
+      <c r="TH43" s="103"/>
+      <c r="TI43" s="103"/>
+      <c r="TJ43" s="103"/>
+      <c r="TK43" s="103"/>
+      <c r="TL43" s="103"/>
+      <c r="TM43" s="103"/>
+      <c r="TN43" s="103"/>
+      <c r="TO43" s="103"/>
+      <c r="TP43" s="103"/>
+      <c r="TQ43" s="103"/>
+      <c r="TR43" s="103"/>
+      <c r="TS43" s="103"/>
+      <c r="TT43" s="103"/>
+      <c r="TU43" s="103"/>
+      <c r="TV43" s="103"/>
+      <c r="TW43" s="103"/>
+      <c r="TX43" s="103"/>
+      <c r="TY43" s="103"/>
+      <c r="TZ43" s="103"/>
+      <c r="UA43" s="103"/>
+      <c r="UB43" s="103"/>
+      <c r="UC43" s="103"/>
+      <c r="UD43" s="103"/>
+      <c r="UE43" s="103"/>
+      <c r="UF43" s="103"/>
+      <c r="UG43" s="103"/>
+      <c r="UH43" s="103"/>
+      <c r="UI43" s="103"/>
+      <c r="UJ43" s="103"/>
+      <c r="UK43" s="103"/>
+      <c r="UL43" s="103"/>
+      <c r="UM43" s="103"/>
+      <c r="UN43" s="103"/>
+      <c r="UO43" s="103"/>
+      <c r="UP43" s="103"/>
+      <c r="UQ43" s="103"/>
+      <c r="UR43" s="103"/>
+      <c r="US43" s="103"/>
+      <c r="UT43" s="103"/>
+      <c r="UU43" s="103"/>
+      <c r="UV43" s="103"/>
+      <c r="UW43" s="103"/>
+      <c r="UX43" s="103"/>
+      <c r="UY43" s="103"/>
+      <c r="UZ43" s="103"/>
+      <c r="VA43" s="103"/>
+      <c r="VB43" s="103"/>
+      <c r="VC43" s="103"/>
+      <c r="VD43" s="103"/>
+      <c r="VE43" s="103"/>
+      <c r="VF43" s="103"/>
+      <c r="VG43" s="103"/>
+      <c r="VH43" s="103"/>
+      <c r="VI43" s="103"/>
+      <c r="VJ43" s="103"/>
+      <c r="VK43" s="103"/>
+      <c r="VL43" s="103"/>
+      <c r="VM43" s="103"/>
+      <c r="VN43" s="103"/>
+      <c r="VO43" s="103"/>
+      <c r="VP43" s="103"/>
+      <c r="VQ43" s="103"/>
+      <c r="VR43" s="103"/>
+      <c r="VS43" s="103"/>
+      <c r="VT43" s="103"/>
+      <c r="VU43" s="103"/>
+      <c r="VV43" s="103"/>
+      <c r="VW43" s="103"/>
+      <c r="VX43" s="103"/>
+      <c r="VY43" s="103"/>
+      <c r="VZ43" s="103"/>
+      <c r="WA43" s="103"/>
+      <c r="WB43" s="103"/>
+      <c r="WC43" s="103"/>
+      <c r="WD43" s="103"/>
+      <c r="WE43" s="103"/>
+      <c r="WF43" s="103"/>
+      <c r="WG43" s="103"/>
+      <c r="WH43" s="103"/>
+      <c r="WI43" s="103"/>
+      <c r="WJ43" s="103"/>
+      <c r="WK43" s="103"/>
+      <c r="WL43" s="103"/>
+      <c r="WM43" s="103"/>
+      <c r="WN43" s="103"/>
+      <c r="WO43" s="103"/>
+      <c r="WP43" s="103"/>
+      <c r="WQ43" s="103"/>
+      <c r="WR43" s="103"/>
+      <c r="WS43" s="103"/>
+      <c r="WT43" s="103"/>
+      <c r="WU43" s="103"/>
+      <c r="WV43" s="103"/>
+      <c r="WW43" s="103"/>
+      <c r="WX43" s="103"/>
+      <c r="WY43" s="103"/>
+      <c r="WZ43" s="103"/>
+      <c r="XA43" s="103"/>
+      <c r="XB43" s="103"/>
+      <c r="XC43" s="103"/>
+      <c r="XD43" s="103"/>
+      <c r="XE43" s="103"/>
+      <c r="XF43" s="103"/>
+      <c r="XG43" s="103"/>
+      <c r="XH43" s="103"/>
+      <c r="XI43" s="103"/>
+      <c r="XJ43" s="103"/>
+      <c r="XK43" s="103"/>
+      <c r="XL43" s="103"/>
+      <c r="XM43" s="103"/>
+      <c r="XN43" s="103"/>
+      <c r="XO43" s="103"/>
+      <c r="XP43" s="103"/>
+      <c r="XQ43" s="103"/>
+      <c r="XR43" s="103"/>
+      <c r="XS43" s="103"/>
+      <c r="XT43" s="103"/>
+      <c r="XU43" s="103"/>
+      <c r="XV43" s="103"/>
+      <c r="XW43" s="103"/>
+      <c r="XX43" s="103"/>
+      <c r="XY43" s="103"/>
+      <c r="XZ43" s="103"/>
+      <c r="YA43" s="103"/>
+      <c r="YB43" s="103"/>
+      <c r="YC43" s="103"/>
+      <c r="YD43" s="103"/>
+      <c r="YE43" s="103"/>
+      <c r="YF43" s="103"/>
+      <c r="YG43" s="103"/>
+      <c r="YH43" s="103"/>
+      <c r="YI43" s="103"/>
+      <c r="YJ43" s="103"/>
+      <c r="YK43" s="103"/>
+      <c r="YL43" s="103"/>
+      <c r="YM43" s="103"/>
+      <c r="YN43" s="103"/>
+      <c r="YO43" s="103"/>
+      <c r="YP43" s="103"/>
+      <c r="YQ43" s="103"/>
+      <c r="YR43" s="103"/>
+      <c r="YS43" s="103"/>
+      <c r="YT43" s="103"/>
+      <c r="YU43" s="103"/>
+      <c r="YV43" s="103"/>
+      <c r="YW43" s="103"/>
+      <c r="YX43" s="103"/>
+      <c r="YY43" s="103"/>
+      <c r="YZ43" s="103"/>
+      <c r="ZA43" s="103"/>
+      <c r="ZB43" s="103"/>
+      <c r="ZC43" s="103"/>
+      <c r="ZD43" s="103"/>
+      <c r="ZE43" s="103"/>
+      <c r="ZF43" s="103"/>
+      <c r="ZG43" s="103"/>
+      <c r="ZH43" s="103"/>
+      <c r="ZI43" s="103"/>
+      <c r="ZJ43" s="103"/>
+      <c r="ZK43" s="103"/>
+      <c r="ZL43" s="103"/>
+      <c r="ZM43" s="103"/>
+      <c r="ZN43" s="103"/>
+      <c r="ZO43" s="103"/>
+      <c r="ZP43" s="103"/>
+      <c r="ZQ43" s="103"/>
+      <c r="ZR43" s="103"/>
+      <c r="ZS43" s="103"/>
+      <c r="ZT43" s="103"/>
+      <c r="ZU43" s="103"/>
+      <c r="ZV43" s="103"/>
+      <c r="ZW43" s="103"/>
+      <c r="ZX43" s="103"/>
+      <c r="ZY43" s="103"/>
+      <c r="ZZ43" s="103"/>
+      <c r="AAA43" s="103"/>
+      <c r="AAB43" s="103"/>
+      <c r="AAC43" s="103"/>
+      <c r="AAD43" s="103"/>
+      <c r="AAE43" s="103"/>
+      <c r="AAF43" s="103"/>
+      <c r="AAG43" s="103"/>
+      <c r="AAH43" s="103"/>
+      <c r="AAI43" s="103"/>
+      <c r="AAJ43" s="103"/>
+      <c r="AAK43" s="103"/>
+      <c r="AAL43" s="103"/>
+      <c r="AAM43" s="103"/>
+      <c r="AAN43" s="103"/>
+      <c r="AAO43" s="103"/>
+      <c r="AAP43" s="103"/>
+      <c r="AAQ43" s="103"/>
+      <c r="AAR43" s="103"/>
+      <c r="AAS43" s="103"/>
+      <c r="AAT43" s="103"/>
+      <c r="AAU43" s="103"/>
+      <c r="AAV43" s="103"/>
+      <c r="AAW43" s="103"/>
+      <c r="AAX43" s="103"/>
+      <c r="AAY43" s="103"/>
+      <c r="AAZ43" s="103"/>
+      <c r="ABA43" s="103"/>
+      <c r="ABB43" s="103"/>
+      <c r="ABC43" s="103"/>
+      <c r="ABD43" s="103"/>
+      <c r="ABE43" s="103"/>
+      <c r="ABF43" s="103"/>
+      <c r="ABG43" s="103"/>
+      <c r="ABH43" s="103"/>
+      <c r="ABI43" s="103"/>
+      <c r="ABJ43" s="103"/>
+      <c r="ABK43" s="103"/>
+      <c r="ABL43" s="103"/>
+      <c r="ABM43" s="103"/>
+      <c r="ABN43" s="103"/>
+      <c r="ABO43" s="103"/>
+      <c r="ABP43" s="103"/>
+      <c r="ABQ43" s="103"/>
+      <c r="ABR43" s="103"/>
+      <c r="ABS43" s="103"/>
+      <c r="ABT43" s="103"/>
+      <c r="ABU43" s="103"/>
+      <c r="ABV43" s="103"/>
+      <c r="ABW43" s="103"/>
+      <c r="ABX43" s="103"/>
+      <c r="ABY43" s="103"/>
+      <c r="ABZ43" s="103"/>
+      <c r="ACA43" s="103"/>
+      <c r="ACB43" s="103"/>
+      <c r="ACC43" s="103"/>
+      <c r="ACD43" s="103"/>
+      <c r="ACE43" s="103"/>
+      <c r="ACF43" s="103"/>
+      <c r="ACG43" s="103"/>
+      <c r="ACH43" s="103"/>
+      <c r="ACI43" s="103"/>
+      <c r="ACJ43" s="103"/>
+      <c r="ACK43" s="103"/>
+      <c r="ACL43" s="103"/>
+      <c r="ACM43" s="103"/>
+      <c r="ACN43" s="103"/>
+      <c r="ACO43" s="103"/>
+      <c r="ACP43" s="103"/>
+      <c r="ACQ43" s="103"/>
+      <c r="ACR43" s="103"/>
+      <c r="ACS43" s="103"/>
+      <c r="ACT43" s="103"/>
+      <c r="ACU43" s="103"/>
+      <c r="ACV43" s="103"/>
+      <c r="ACW43" s="103"/>
+      <c r="ACX43" s="103"/>
+      <c r="ACY43" s="103"/>
+      <c r="ACZ43" s="103"/>
+      <c r="ADA43" s="103"/>
+      <c r="ADB43" s="103"/>
+      <c r="ADC43" s="103"/>
+      <c r="ADD43" s="103"/>
+      <c r="ADE43" s="103"/>
+      <c r="ADF43" s="103"/>
+      <c r="ADG43" s="103"/>
+      <c r="ADH43" s="103"/>
+      <c r="ADI43" s="103"/>
+      <c r="ADJ43" s="103"/>
+      <c r="ADK43" s="103"/>
+      <c r="ADL43" s="103"/>
+      <c r="ADM43" s="103"/>
+      <c r="ADN43" s="103"/>
+      <c r="ADO43" s="103"/>
+      <c r="ADP43" s="103"/>
+      <c r="ADQ43" s="103"/>
+      <c r="ADR43" s="103"/>
+      <c r="ADS43" s="103"/>
+      <c r="ADT43" s="103"/>
+      <c r="ADU43" s="103"/>
+      <c r="ADV43" s="103"/>
+      <c r="ADW43" s="103"/>
+      <c r="ADX43" s="103"/>
+      <c r="ADY43" s="103"/>
+      <c r="ADZ43" s="103"/>
+      <c r="AEA43" s="103"/>
+      <c r="AEB43" s="103"/>
+      <c r="AEC43" s="103"/>
+      <c r="AED43" s="103"/>
+      <c r="AEE43" s="103"/>
+      <c r="AEF43" s="103"/>
+      <c r="AEG43" s="103"/>
+      <c r="AEH43" s="103"/>
+      <c r="AEI43" s="103"/>
+      <c r="AEJ43" s="103"/>
+      <c r="AEK43" s="103"/>
+      <c r="AEL43" s="103"/>
+      <c r="AEM43" s="103"/>
+      <c r="AEN43" s="103"/>
+      <c r="AEO43" s="103"/>
+      <c r="AEP43" s="103"/>
+      <c r="AEQ43" s="103"/>
+      <c r="AER43" s="103"/>
+      <c r="AES43" s="103"/>
+      <c r="AET43" s="103"/>
+      <c r="AEU43" s="103"/>
+      <c r="AEV43" s="103"/>
+      <c r="AEW43" s="103"/>
+      <c r="AEX43" s="103"/>
+      <c r="AEY43" s="103"/>
+      <c r="AEZ43" s="103"/>
+      <c r="AFA43" s="103"/>
+      <c r="AFB43" s="103"/>
+      <c r="AFC43" s="103"/>
+      <c r="AFD43" s="103"/>
+      <c r="AFE43" s="103"/>
+      <c r="AFF43" s="103"/>
+      <c r="AFG43" s="103"/>
+      <c r="AFH43" s="103"/>
+      <c r="AFI43" s="103"/>
+      <c r="AFJ43" s="103"/>
+      <c r="AFK43" s="103"/>
+      <c r="AFL43" s="103"/>
+      <c r="AFM43" s="103"/>
+      <c r="AFN43" s="103"/>
+      <c r="AFO43" s="103"/>
+      <c r="AFP43" s="103"/>
+      <c r="AFQ43" s="103"/>
+      <c r="AFR43" s="103"/>
+      <c r="AFS43" s="103"/>
+      <c r="AFT43" s="103"/>
+      <c r="AFU43" s="103"/>
+      <c r="AFV43" s="103"/>
+      <c r="AFW43" s="103"/>
+      <c r="AFX43" s="103"/>
+      <c r="AFY43" s="103"/>
+      <c r="AFZ43" s="103"/>
+      <c r="AGA43" s="103"/>
+      <c r="AGB43" s="103"/>
+      <c r="AGC43" s="103"/>
+      <c r="AGD43" s="103"/>
+      <c r="AGE43" s="103"/>
+      <c r="AGF43" s="103"/>
+      <c r="AGG43" s="103"/>
+      <c r="AGH43" s="103"/>
+      <c r="AGI43" s="103"/>
+      <c r="AGJ43" s="103"/>
+      <c r="AGK43" s="103"/>
+      <c r="AGL43" s="103"/>
+      <c r="AGM43" s="103"/>
+      <c r="AGN43" s="103"/>
+      <c r="AGO43" s="103"/>
+      <c r="AGP43" s="103"/>
+      <c r="AGQ43" s="103"/>
+      <c r="AGR43" s="103"/>
+      <c r="AGS43" s="103"/>
+      <c r="AGT43" s="103"/>
+      <c r="AGU43" s="103"/>
+      <c r="AGV43" s="103"/>
+      <c r="AGW43" s="103"/>
+      <c r="AGX43" s="103"/>
+      <c r="AGY43" s="103"/>
+      <c r="AGZ43" s="103"/>
+      <c r="AHA43" s="103"/>
+      <c r="AHB43" s="103"/>
+      <c r="AHC43" s="103"/>
+      <c r="AHD43" s="103"/>
+      <c r="AHE43" s="103"/>
+      <c r="AHF43" s="103"/>
+      <c r="AHG43" s="103"/>
+      <c r="AHH43" s="103"/>
+      <c r="AHI43" s="103"/>
+      <c r="AHJ43" s="103"/>
+      <c r="AHK43" s="103"/>
+      <c r="AHL43" s="103"/>
+      <c r="AHM43" s="103"/>
+      <c r="AHN43" s="103"/>
+      <c r="AHO43" s="103"/>
+      <c r="AHP43" s="103"/>
+      <c r="AHQ43" s="103"/>
+      <c r="AHR43" s="103"/>
+      <c r="AHS43" s="103"/>
+      <c r="AHT43" s="103"/>
+      <c r="AHU43" s="103"/>
+      <c r="AHV43" s="103"/>
+      <c r="AHW43" s="103"/>
+      <c r="AHX43" s="103"/>
+      <c r="AHY43" s="103"/>
+      <c r="AHZ43" s="103"/>
+      <c r="AIA43" s="103"/>
+      <c r="AIB43" s="103"/>
+      <c r="AIC43" s="103"/>
+      <c r="AID43" s="103"/>
+      <c r="AIE43" s="103"/>
+      <c r="AIF43" s="103"/>
+      <c r="AIG43" s="103"/>
+      <c r="AIH43" s="103"/>
+      <c r="AII43" s="103"/>
+      <c r="AIJ43" s="103"/>
+      <c r="AIK43" s="103"/>
+      <c r="AIL43" s="103"/>
+      <c r="AIM43" s="103"/>
+      <c r="AIN43" s="103"/>
+      <c r="AIO43" s="103"/>
+      <c r="AIP43" s="103"/>
+      <c r="AIQ43" s="103"/>
+      <c r="AIR43" s="103"/>
+      <c r="AIS43" s="103"/>
+      <c r="AIT43" s="103"/>
+      <c r="AIU43" s="103"/>
+      <c r="AIV43" s="103"/>
+      <c r="AIW43" s="103"/>
+      <c r="AIX43" s="103"/>
+      <c r="AIY43" s="103"/>
+      <c r="AIZ43" s="103"/>
+      <c r="AJA43" s="103"/>
+      <c r="AJB43" s="103"/>
+      <c r="AJC43" s="103"/>
+      <c r="AJD43" s="103"/>
+      <c r="AJE43" s="103"/>
+      <c r="AJF43" s="103"/>
+      <c r="AJG43" s="103"/>
+      <c r="AJH43" s="103"/>
+      <c r="AJI43" s="103"/>
+      <c r="AJJ43" s="103"/>
+      <c r="AJK43" s="103"/>
+      <c r="AJL43" s="103"/>
+      <c r="AJM43" s="103"/>
+      <c r="AJN43" s="103"/>
+      <c r="AJO43" s="103"/>
+      <c r="AJP43" s="103"/>
+      <c r="AJQ43" s="103"/>
+      <c r="AJR43" s="103"/>
+      <c r="AJS43" s="103"/>
+      <c r="AJT43" s="103"/>
+      <c r="AJU43" s="103"/>
+      <c r="AJV43" s="103"/>
+      <c r="AJW43" s="103"/>
+      <c r="AJX43" s="103"/>
+      <c r="AJY43" s="103"/>
+      <c r="AJZ43" s="103"/>
+      <c r="AKA43" s="103"/>
+      <c r="AKB43" s="103"/>
+      <c r="AKC43" s="103"/>
+      <c r="AKD43" s="103"/>
+      <c r="AKE43" s="103"/>
+      <c r="AKF43" s="103"/>
+      <c r="AKG43" s="103"/>
+      <c r="AKH43" s="103"/>
+      <c r="AKI43" s="103"/>
+      <c r="AKJ43" s="103"/>
+      <c r="AKK43" s="103"/>
+      <c r="AKL43" s="103"/>
+      <c r="AKM43" s="103"/>
+      <c r="AKN43" s="103"/>
+      <c r="AKO43" s="103"/>
+      <c r="AKP43" s="103"/>
+      <c r="AKQ43" s="103"/>
+      <c r="AKR43" s="103"/>
+      <c r="AKS43" s="103"/>
+      <c r="AKT43" s="103"/>
+      <c r="AKU43" s="103"/>
+      <c r="AKV43" s="103"/>
+      <c r="AKW43" s="103"/>
+      <c r="AKX43" s="103"/>
+      <c r="AKY43" s="103"/>
+      <c r="AKZ43" s="103"/>
+      <c r="ALA43" s="103"/>
+      <c r="ALB43" s="103"/>
+      <c r="ALC43" s="103"/>
+      <c r="ALD43" s="103"/>
+      <c r="ALE43" s="103"/>
+      <c r="ALF43" s="103"/>
+      <c r="ALG43" s="103"/>
+      <c r="ALH43" s="103"/>
+      <c r="ALI43" s="103"/>
+      <c r="ALJ43" s="103"/>
+      <c r="ALK43" s="103"/>
+      <c r="ALL43" s="103"/>
+      <c r="ALM43" s="103"/>
+      <c r="ALN43" s="103"/>
+      <c r="ALO43" s="103"/>
+      <c r="ALP43" s="103"/>
+      <c r="ALQ43" s="103"/>
+      <c r="ALR43" s="103"/>
+      <c r="ALS43" s="103"/>
+      <c r="ALT43" s="103"/>
+      <c r="ALU43" s="103"/>
+      <c r="ALV43" s="103"/>
+      <c r="ALW43" s="103"/>
+      <c r="ALX43" s="103"/>
+      <c r="ALY43" s="103"/>
+      <c r="ALZ43" s="103"/>
+      <c r="AMA43" s="103"/>
+      <c r="AMB43" s="103"/>
+      <c r="AMC43" s="103"/>
+      <c r="AMD43" s="103"/>
+      <c r="AME43" s="103"/>
+      <c r="AMF43" s="103"/>
+      <c r="AMG43" s="103"/>
+      <c r="AMH43" s="103"/>
+      <c r="AMI43" s="103"/>
+      <c r="AMJ43" s="103"/>
+      <c r="AMK43" s="103"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="B44" s="32"/>
       <c r="C44" s="32"/>
       <c r="D44" s="32"/>
@@ -4174,7 +5232,7 @@
       <c r="O44" s="32"/>
       <c r="P44" s="32"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
@@ -4191,7 +5249,7 @@
       <c r="O45" s="32"/>
       <c r="P45" s="32"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="B46" s="32"/>
       <c r="C46" s="32"/>
       <c r="D46" s="32"/>
@@ -4208,7 +5266,7 @@
       <c r="O46" s="32"/>
       <c r="P46" s="32"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1025" x14ac:dyDescent="0.35">
       <c r="B47" s="32"/>
       <c r="C47" s="32"/>
       <c r="D47" s="32"/>
@@ -4236,8 +5294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4602,302 +5660,302 @@
       <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="93" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="97">
+      <c r="B8" s="92">
         <v>2</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="92">
         <v>13</v>
       </c>
-      <c r="D8" s="97">
+      <c r="D8" s="92">
         <v>27</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="92">
         <v>5</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="92">
         <v>12</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G8" s="92">
         <v>42</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="92">
         <v>68</v>
       </c>
-      <c r="I8" s="97">
+      <c r="I8" s="92">
         <v>85</v>
       </c>
-      <c r="J8" s="97">
+      <c r="J8" s="92">
         <v>140</v>
       </c>
-      <c r="K8" s="97">
+      <c r="K8" s="92">
         <v>87</v>
       </c>
-      <c r="L8" s="97">
+      <c r="L8" s="92">
         <v>99</v>
       </c>
-      <c r="M8" s="97">
+      <c r="M8" s="92">
         <v>116</v>
       </c>
-      <c r="N8" s="97">
+      <c r="N8" s="92">
         <v>157</v>
       </c>
-      <c r="O8" s="97">
+      <c r="O8" s="92">
         <v>264</v>
       </c>
-      <c r="P8" s="97">
+      <c r="P8" s="92">
         <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="97">
+      <c r="B9" s="92">
         <v>1</v>
       </c>
-      <c r="C9" s="97">
+      <c r="C9" s="92">
         <v>1</v>
       </c>
-      <c r="D9" s="97">
+      <c r="D9" s="92">
         <v>0</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E9" s="92">
         <v>1</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F9" s="92">
         <v>3</v>
       </c>
-      <c r="G9" s="97">
+      <c r="G9" s="92">
         <v>2</v>
       </c>
-      <c r="H9" s="97">
+      <c r="H9" s="92">
         <v>7</v>
       </c>
-      <c r="I9" s="97">
+      <c r="I9" s="92">
         <v>14</v>
       </c>
-      <c r="J9" s="97">
+      <c r="J9" s="92">
         <v>19</v>
       </c>
-      <c r="K9" s="97">
+      <c r="K9" s="92">
         <v>9</v>
       </c>
-      <c r="L9" s="97">
+      <c r="L9" s="92">
         <v>11</v>
       </c>
-      <c r="M9" s="97">
+      <c r="M9" s="92">
         <v>15</v>
       </c>
-      <c r="N9" s="97">
+      <c r="N9" s="92">
         <v>28</v>
       </c>
-      <c r="O9" s="97">
+      <c r="O9" s="92">
         <v>44</v>
       </c>
-      <c r="P9" s="97">
+      <c r="P9" s="92">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="97">
+      <c r="B10" s="92">
         <v>0</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="92">
         <v>0</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="92">
         <v>0</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="92">
         <v>0</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="92">
         <v>0</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="92">
         <v>2</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H10" s="92">
         <v>2</v>
       </c>
-      <c r="I10" s="97">
+      <c r="I10" s="92">
         <v>1</v>
       </c>
-      <c r="J10" s="97">
+      <c r="J10" s="92">
         <v>1</v>
       </c>
-      <c r="K10" s="97">
+      <c r="K10" s="92">
         <v>2</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="92">
         <v>4</v>
       </c>
-      <c r="M10" s="97">
+      <c r="M10" s="92">
         <v>5</v>
       </c>
-      <c r="N10" s="97">
+      <c r="N10" s="92">
         <v>4</v>
       </c>
-      <c r="O10" s="97">
+      <c r="O10" s="92">
         <v>3</v>
       </c>
-      <c r="P10" s="97">
+      <c r="P10" s="92">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="92">
         <v>0</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="92">
         <v>0</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="92">
         <v>0</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="92">
         <v>0</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="92">
         <v>0</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="92">
         <v>1</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="92">
         <v>0</v>
       </c>
-      <c r="I11" s="97">
+      <c r="I11" s="92">
         <v>0</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J11" s="92">
         <v>0</v>
       </c>
-      <c r="K11" s="97">
+      <c r="K11" s="92">
         <v>0</v>
       </c>
-      <c r="L11" s="97">
+      <c r="L11" s="92">
         <v>0</v>
       </c>
-      <c r="M11" s="97">
+      <c r="M11" s="92">
         <v>1</v>
       </c>
-      <c r="N11" s="97">
+      <c r="N11" s="92">
         <v>0</v>
       </c>
-      <c r="O11" s="97">
+      <c r="O11" s="92">
         <v>0</v>
       </c>
-      <c r="P11" s="97">
+      <c r="P11" s="92">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="97">
+      <c r="B12" s="92">
         <v>5</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="92">
         <v>29</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D12" s="92">
         <v>41</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="92">
         <v>6</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="92">
         <v>12</v>
       </c>
-      <c r="G12" s="97">
+      <c r="G12" s="92">
         <v>43</v>
       </c>
-      <c r="H12" s="97">
+      <c r="H12" s="92">
         <v>79</v>
       </c>
-      <c r="I12" s="97">
+      <c r="I12" s="92">
         <v>111</v>
       </c>
-      <c r="J12" s="97">
+      <c r="J12" s="92">
         <v>132</v>
       </c>
-      <c r="K12" s="97">
+      <c r="K12" s="92">
         <v>104</v>
       </c>
-      <c r="L12" s="97">
+      <c r="L12" s="92">
         <v>112</v>
       </c>
-      <c r="M12" s="97">
+      <c r="M12" s="92">
         <v>118</v>
       </c>
-      <c r="N12" s="97">
+      <c r="N12" s="92">
         <v>190</v>
       </c>
-      <c r="O12" s="97">
+      <c r="O12" s="92">
         <v>319</v>
       </c>
-      <c r="P12" s="97">
+      <c r="P12" s="92">
         <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="97">
+      <c r="B13" s="92">
         <v>0</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="92">
         <v>0</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D13" s="92">
         <v>0</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="92">
         <v>0</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F13" s="92">
         <v>1</v>
       </c>
-      <c r="G13" s="97">
+      <c r="G13" s="92">
         <v>1</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H13" s="92">
         <v>0</v>
       </c>
-      <c r="I13" s="97">
+      <c r="I13" s="92">
         <v>1</v>
       </c>
-      <c r="J13" s="97">
+      <c r="J13" s="92">
         <v>1</v>
       </c>
-      <c r="K13" s="97">
+      <c r="K13" s="92">
         <v>0</v>
       </c>
-      <c r="L13" s="97">
+      <c r="L13" s="92">
         <v>1</v>
       </c>
-      <c r="M13" s="97">
+      <c r="M13" s="92">
         <v>0</v>
       </c>
-      <c r="N13" s="97">
+      <c r="N13" s="92">
         <v>4</v>
       </c>
-      <c r="O13" s="97">
+      <c r="O13" s="92">
         <v>6</v>
       </c>
-      <c r="P13" s="97">
+      <c r="P13" s="92">
         <v>7</v>
       </c>
     </row>
@@ -5611,6 +6669,14 @@
       </c>
       <c r="E42" s="32">
         <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="102" t="s">
+        <v>210</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
@@ -6117,49 +7183,49 @@
       <c r="A10" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="97">
+      <c r="B10" s="92">
         <v>0</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="92">
         <v>2</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="92">
         <v>0</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="92">
         <v>0</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="92">
         <v>0</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="92">
         <v>1</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H10" s="92">
         <v>1</v>
       </c>
-      <c r="I10" s="97">
+      <c r="I10" s="92">
         <v>1</v>
       </c>
-      <c r="J10" s="97">
+      <c r="J10" s="92">
         <v>1</v>
       </c>
-      <c r="K10" s="97">
+      <c r="K10" s="92">
         <v>1</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="92">
         <v>1</v>
       </c>
-      <c r="M10" s="97">
+      <c r="M10" s="92">
         <v>3</v>
       </c>
-      <c r="N10" s="97">
+      <c r="N10" s="92">
         <v>2</v>
       </c>
-      <c r="O10" s="97">
+      <c r="O10" s="92">
         <v>7</v>
       </c>
-      <c r="P10" s="97">
+      <c r="P10" s="92">
         <v>6</v>
       </c>
     </row>
@@ -6167,49 +7233,49 @@
       <c r="A11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="92">
         <v>0</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="92">
         <v>0</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="92">
         <v>0</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="92">
         <v>0</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="92">
         <v>0</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="92">
         <v>0</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="92">
         <v>0</v>
       </c>
-      <c r="I11" s="97">
+      <c r="I11" s="92">
         <v>0</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J11" s="92">
         <v>0</v>
       </c>
-      <c r="K11" s="97">
+      <c r="K11" s="92">
         <v>0</v>
       </c>
-      <c r="L11" s="97">
+      <c r="L11" s="92">
         <v>0</v>
       </c>
-      <c r="M11" s="97">
+      <c r="M11" s="92">
         <v>0</v>
       </c>
-      <c r="N11" s="97">
+      <c r="N11" s="92">
         <v>0</v>
       </c>
-      <c r="O11" s="97">
+      <c r="O11" s="92">
         <v>0</v>
       </c>
-      <c r="P11" s="97">
+      <c r="P11" s="92">
         <v>1</v>
       </c>
     </row>
@@ -7049,8 +8115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D94F6E-ADED-482F-8CE6-830729D726B5}">
   <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7416,49 +8482,49 @@
       <c r="A8" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="97">
+      <c r="B8" s="92">
         <v>3</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="92">
         <v>21</v>
       </c>
-      <c r="D8" s="97">
+      <c r="D8" s="92">
         <v>30</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="92">
         <v>9</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="92">
         <v>8</v>
       </c>
-      <c r="G8" s="97">
+      <c r="G8" s="92">
         <v>42</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="92">
         <v>106</v>
       </c>
-      <c r="I8" s="97">
+      <c r="I8" s="92">
         <v>90</v>
       </c>
-      <c r="J8" s="97">
+      <c r="J8" s="92">
         <v>133</v>
       </c>
-      <c r="K8" s="97">
+      <c r="K8" s="92">
         <v>126</v>
       </c>
-      <c r="L8" s="97">
+      <c r="L8" s="92">
         <v>125</v>
       </c>
-      <c r="M8" s="97">
+      <c r="M8" s="92">
         <v>147</v>
       </c>
-      <c r="N8" s="97">
+      <c r="N8" s="92">
         <v>165</v>
       </c>
-      <c r="O8" s="97">
+      <c r="O8" s="92">
         <v>248</v>
       </c>
-      <c r="P8" s="97">
+      <c r="P8" s="92">
         <v>314</v>
       </c>
       <c r="Q8" s="37"/>
@@ -7468,49 +8534,49 @@
       <c r="A9" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="97">
+      <c r="B9" s="92">
         <v>1</v>
       </c>
-      <c r="C9" s="97">
+      <c r="C9" s="92">
         <v>1</v>
       </c>
-      <c r="D9" s="97">
+      <c r="D9" s="92">
         <v>0</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E9" s="92">
         <v>1</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F9" s="92">
         <v>0</v>
       </c>
-      <c r="G9" s="97">
+      <c r="G9" s="92">
         <v>1</v>
       </c>
-      <c r="H9" s="97">
+      <c r="H9" s="92">
         <v>8</v>
       </c>
-      <c r="I9" s="97">
+      <c r="I9" s="92">
         <v>18</v>
       </c>
-      <c r="J9" s="97">
+      <c r="J9" s="92">
         <v>14</v>
       </c>
-      <c r="K9" s="97">
+      <c r="K9" s="92">
         <v>8</v>
       </c>
-      <c r="L9" s="97">
+      <c r="L9" s="92">
         <v>14</v>
       </c>
-      <c r="M9" s="97">
+      <c r="M9" s="92">
         <v>15</v>
       </c>
-      <c r="N9" s="97">
+      <c r="N9" s="92">
         <v>13</v>
       </c>
-      <c r="O9" s="97">
+      <c r="O9" s="92">
         <v>22</v>
       </c>
-      <c r="P9" s="97">
+      <c r="P9" s="92">
         <v>31</v>
       </c>
       <c r="Q9" s="37"/>
@@ -7520,49 +8586,49 @@
       <c r="A10" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="97">
+      <c r="B10" s="92">
         <v>0</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="92">
         <v>0</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="92">
         <v>0</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="92">
         <v>0</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="92">
         <v>0</v>
       </c>
-      <c r="G10" s="97">
+      <c r="G10" s="92">
         <v>0</v>
       </c>
-      <c r="H10" s="97">
+      <c r="H10" s="92">
         <v>2</v>
       </c>
-      <c r="I10" s="97">
+      <c r="I10" s="92">
         <v>0</v>
       </c>
-      <c r="J10" s="97">
+      <c r="J10" s="92">
         <v>0</v>
       </c>
-      <c r="K10" s="97">
+      <c r="K10" s="92">
         <v>0</v>
       </c>
-      <c r="L10" s="97">
+      <c r="L10" s="92">
         <v>0</v>
       </c>
-      <c r="M10" s="97">
+      <c r="M10" s="92">
         <v>1</v>
       </c>
-      <c r="N10" s="97">
+      <c r="N10" s="92">
         <v>0</v>
       </c>
-      <c r="O10" s="97">
+      <c r="O10" s="92">
         <v>1</v>
       </c>
-      <c r="P10" s="97">
+      <c r="P10" s="92">
         <v>2</v>
       </c>
       <c r="Q10" s="37"/>
@@ -7572,49 +8638,49 @@
       <c r="A11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="97">
+      <c r="B11" s="92">
         <v>0</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="92">
         <v>0</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="92">
         <v>0</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="92">
         <v>0</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="92">
         <v>0</v>
       </c>
-      <c r="G11" s="97">
+      <c r="G11" s="92">
         <v>0</v>
       </c>
-      <c r="H11" s="97">
+      <c r="H11" s="92">
         <v>0</v>
       </c>
-      <c r="I11" s="97">
+      <c r="I11" s="92">
         <v>0</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J11" s="92">
         <v>0</v>
       </c>
-      <c r="K11" s="97">
+      <c r="K11" s="92">
         <v>0</v>
       </c>
-      <c r="L11" s="97">
+      <c r="L11" s="92">
         <v>0</v>
       </c>
-      <c r="M11" s="97">
+      <c r="M11" s="92">
         <v>0</v>
       </c>
-      <c r="N11" s="97">
+      <c r="N11" s="92">
         <v>0</v>
       </c>
-      <c r="O11" s="97">
+      <c r="O11" s="92">
         <v>0</v>
       </c>
-      <c r="P11" s="97">
+      <c r="P11" s="92">
         <v>0</v>
       </c>
       <c r="Y11" s="37"/>
@@ -7638,49 +8704,49 @@
       <c r="A12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="97">
+      <c r="B12" s="92">
         <v>7</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="92">
         <v>24</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D12" s="92">
         <v>42</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="92">
         <v>10</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="92">
         <v>8</v>
       </c>
-      <c r="G12" s="97">
+      <c r="G12" s="92">
         <v>46</v>
       </c>
-      <c r="H12" s="97">
+      <c r="H12" s="92">
         <v>103</v>
       </c>
-      <c r="I12" s="97">
+      <c r="I12" s="92">
         <v>137</v>
       </c>
-      <c r="J12" s="97">
+      <c r="J12" s="92">
         <v>168</v>
       </c>
-      <c r="K12" s="97">
+      <c r="K12" s="92">
         <v>169</v>
       </c>
-      <c r="L12" s="97">
+      <c r="L12" s="92">
         <v>208</v>
       </c>
-      <c r="M12" s="97">
+      <c r="M12" s="92">
         <v>184</v>
       </c>
-      <c r="N12" s="97">
+      <c r="N12" s="92">
         <v>213</v>
       </c>
-      <c r="O12" s="97">
+      <c r="O12" s="92">
         <v>400</v>
       </c>
-      <c r="P12" s="97">
+      <c r="P12" s="92">
         <v>459</v>
       </c>
       <c r="Y12" s="37"/>
@@ -7704,49 +8770,49 @@
       <c r="A13" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="97">
+      <c r="B13" s="92">
         <v>0</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="92">
         <v>0</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D13" s="92">
         <v>0</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="92">
         <v>0</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F13" s="92">
         <v>0</v>
       </c>
-      <c r="G13" s="97">
+      <c r="G13" s="92">
         <v>0</v>
       </c>
-      <c r="H13" s="97">
+      <c r="H13" s="92">
         <v>0</v>
       </c>
-      <c r="I13" s="97">
+      <c r="I13" s="92">
         <v>1</v>
       </c>
-      <c r="J13" s="97">
+      <c r="J13" s="92">
         <v>1</v>
       </c>
-      <c r="K13" s="97">
+      <c r="K13" s="92">
         <v>0</v>
       </c>
-      <c r="L13" s="97">
+      <c r="L13" s="92">
         <v>1</v>
       </c>
-      <c r="M13" s="97">
+      <c r="M13" s="92">
         <v>1</v>
       </c>
-      <c r="N13" s="97">
+      <c r="N13" s="92">
         <v>2</v>
       </c>
-      <c r="O13" s="97">
+      <c r="O13" s="92">
         <v>6</v>
       </c>
-      <c r="P13" s="97">
+      <c r="P13" s="92">
         <v>6</v>
       </c>
       <c r="Y13" s="37"/>
@@ -7915,7 +8981,7 @@
         <f>1468/10736</f>
         <v>0.13673621460506707</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="94" t="s">
         <v>202</v>
       </c>
       <c r="D17" s="36"/>
@@ -8453,7 +9519,7 @@
       <c r="A37" s="88" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="100">
+      <c r="B37" s="95">
         <f>21+20</f>
         <v>41</v>
       </c>
@@ -8483,7 +9549,7 @@
       <c r="A38" s="88" t="s">
         <v>201</v>
       </c>
-      <c r="B38" s="100">
+      <c r="B38" s="95">
         <f>3+5</f>
         <v>8</v>
       </c>
@@ -8521,7 +9587,7 @@
       <c r="D39" s="72">
         <v>157</v>
       </c>
-      <c r="E39" s="101">
+      <c r="E39" s="96">
         <v>340</v>
       </c>
       <c r="F39" s="32"/>
@@ -8549,7 +9615,7 @@
       <c r="D40" s="72">
         <v>32</v>
       </c>
-      <c r="E40" s="101">
+      <c r="E40" s="96">
         <v>54</v>
       </c>
       <c r="F40" s="32"/>
@@ -8630,7 +9696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2F92BF-FD62-4896-B0D4-509004DB7F1D}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -9320,17 +10386,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
@@ -9626,10 +10692,10 @@
       <c r="D19" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="93"/>
+      <c r="F19" s="98"/>
       <c r="G19" s="47" t="s">
         <v>93</v>
       </c>
@@ -9656,11 +10722,11 @@
       <c r="D20" s="44">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="99">
         <f>G16/(B21*E7+C21*F7+D21)</f>
         <v>7.3142891277727717E-2</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="100"/>
       <c r="G20" s="57">
         <f>E7*E20</f>
         <v>0.11215243329251584</v>
@@ -9698,12 +10764,12 @@
         <f>D20/(B20+C20+D20)</f>
         <v>0.3109756097560975</v>
       </c>
-      <c r="E21" s="96" t="s">
+      <c r="E21" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="96"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
       <c r="I21" s="46" t="s">
         <v>112</v>
       </c>
@@ -9712,10 +10778,10 @@
       <c r="B22" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="93"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="47" t="s">
         <v>101</v>
       </c>
@@ -9724,11 +10790,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E23" s="94">
+      <c r="E23" s="99">
         <f>I16/(B21*E7+C21*F7+D21)</f>
         <v>6.1994547887484576E-2</v>
       </c>
-      <c r="F23" s="95"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="57">
         <f>E7*E23</f>
         <v>9.5058306760809688E-2</v>
@@ -9739,12 +10805,12 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E24" s="92" t="s">
+      <c r="E24" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E25" s="65"/>
@@ -9927,10 +10993,10 @@
       <c r="D35" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="93" t="s">
+      <c r="E35" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="93"/>
+      <c r="F35" s="98"/>
       <c r="G35" s="47" t="s">
         <v>99</v>
       </c>
@@ -9957,11 +11023,11 @@
       <c r="D36" s="38">
         <v>0.10100000000000001</v>
       </c>
-      <c r="E36" s="94">
+      <c r="E36" s="99">
         <f>G32/(B37*E7+C37*F7+D37)</f>
         <v>0.10569993007107925</v>
       </c>
-      <c r="F36" s="95"/>
+      <c r="F36" s="100"/>
       <c r="G36" s="57">
         <f>E7*E36</f>
         <v>0.16207322610898819</v>
@@ -9999,12 +11065,12 @@
         <f>D36/(B36+C36+D36)</f>
         <v>0.47867298578199052</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="96"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
       <c r="I37" s="46" t="s">
         <v>112</v>
       </c>
@@ -10013,10 +11079,10 @@
       <c r="B38" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="93" t="s">
+      <c r="E38" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="93"/>
+      <c r="F38" s="98"/>
       <c r="G38" s="47" t="s">
         <v>101</v>
       </c>
@@ -10025,11 +11091,11 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E39" s="94">
+      <c r="E39" s="99">
         <f>I32/(B37*E7+C37*F7+D37)</f>
         <v>6.7659676993794202E-2</v>
       </c>
-      <c r="F39" s="95"/>
+      <c r="F39" s="100"/>
       <c r="G39" s="57">
         <f>E7*E39</f>
         <v>0.10374483805715112</v>
@@ -10040,12 +11106,12 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="96"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="96"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="101"/>
     </row>
     <row r="43" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="59" t="s">
@@ -10222,10 +11288,10 @@
       <c r="D51" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E51" s="93" t="s">
+      <c r="E51" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="93"/>
+      <c r="F51" s="98"/>
       <c r="G51" s="47" t="s">
         <v>99</v>
       </c>
@@ -10252,11 +11318,11 @@
       <c r="D52" s="38">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="E52" s="94">
+      <c r="E52" s="99">
         <f>G48/(B53*E7+C53*F7+D53)</f>
         <v>0.18549124507971645</v>
       </c>
-      <c r="F52" s="95"/>
+      <c r="F52" s="100"/>
       <c r="G52" s="57">
         <f>E7*E52</f>
         <v>0.28441990912223192</v>
@@ -10294,12 +11360,12 @@
         <f>D52/(B52+C52+D52)</f>
         <v>0.57534246575342463</v>
       </c>
-      <c r="E53" s="96" t="s">
+      <c r="E53" s="101" t="s">
         <v>187</v>
       </c>
-      <c r="F53" s="96"/>
-      <c r="G53" s="96"/>
-      <c r="H53" s="96"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="101"/>
+      <c r="H53" s="101"/>
       <c r="I53" s="46" t="s">
         <v>112</v>
       </c>
@@ -10308,10 +11374,10 @@
       <c r="B54" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="93" t="s">
+      <c r="E54" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F54" s="93"/>
+      <c r="F54" s="98"/>
       <c r="G54" s="47" t="s">
         <v>101</v>
       </c>
@@ -10320,11 +11386,11 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E55" s="94">
+      <c r="E55" s="99">
         <f>I48/(B53*E7+C53*F7+D53)</f>
         <v>0.10205774331564993</v>
       </c>
-      <c r="F55" s="95"/>
+      <c r="F55" s="100"/>
       <c r="G55" s="57">
         <f>E7*E55</f>
         <v>0.15648853975066324</v>
@@ -10335,12 +11401,12 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E56" s="96" t="s">
+      <c r="E56" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="F56" s="96"/>
-      <c r="G56" s="96"/>
-      <c r="H56" s="96"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="101"/>
+      <c r="H56" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -10393,17 +11459,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="62" t="s">
@@ -10698,10 +11764,10 @@
       <c r="D19" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="93"/>
+      <c r="F19" s="98"/>
       <c r="G19" s="69" t="s">
         <v>93</v>
       </c>
@@ -10728,11 +11794,11 @@
       <c r="D20" s="44">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="99">
         <f>G16/(B21*E7+C21*F7+D21)</f>
         <v>10.440739065375306</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="100"/>
       <c r="G20" s="70">
         <f>E7*E20</f>
         <v>10.440739065375306</v>
@@ -10770,12 +11836,12 @@
         <f>D20/(B20+C20+D20)</f>
         <v>0.3109756097560975</v>
       </c>
-      <c r="E21" s="96" t="s">
+      <c r="E21" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="96"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
       <c r="I21" s="46" t="s">
         <v>112</v>
       </c>
@@ -10784,10 +11850,10 @@
       <c r="B22" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="93"/>
+      <c r="F22" s="98"/>
       <c r="G22" s="69" t="s">
         <v>101</v>
       </c>
@@ -10796,11 +11862,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E23" s="94">
+      <c r="E23" s="99">
         <f>I16/(B21*E7+C21*F7+D21)</f>
         <v>8.5411272906036757</v>
       </c>
-      <c r="F23" s="95"/>
+      <c r="F23" s="100"/>
       <c r="G23" s="70">
         <f>E7*E23</f>
         <v>8.5411272906036757</v>
@@ -10811,12 +11877,12 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E24" s="92" t="s">
+      <c r="E24" s="97" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E25" s="68"/>
@@ -11001,10 +12067,10 @@
       <c r="D35" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="93" t="s">
+      <c r="E35" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="93"/>
+      <c r="F35" s="98"/>
       <c r="G35" s="69" t="s">
         <v>99</v>
       </c>
@@ -11031,11 +12097,11 @@
       <c r="D36" s="38">
         <v>0.10100000000000001</v>
       </c>
-      <c r="E36" s="94">
+      <c r="E36" s="99">
         <f>G32/(B37*E7+C37*F7+D37)</f>
         <v>17.40345441898717</v>
       </c>
-      <c r="F36" s="95"/>
+      <c r="F36" s="100"/>
       <c r="G36" s="70">
         <f>E7*E36</f>
         <v>17.40345441898717</v>
@@ -11073,12 +12139,12 @@
         <f>D36/(B36+C36+D36)</f>
         <v>0.47867298578199052</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="96"/>
+      <c r="F37" s="101"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="101"/>
       <c r="I37" s="46" t="s">
         <v>112</v>
       </c>
@@ -11087,10 +12153,10 @@
       <c r="B38" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E38" s="93" t="s">
+      <c r="E38" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="93"/>
+      <c r="F38" s="98"/>
       <c r="G38" s="69" t="s">
         <v>101</v>
       </c>
@@ -11099,11 +12165,11 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E39" s="94">
+      <c r="E39" s="99">
         <f>I32/(B37*E7+C37*F7+D37)</f>
         <v>8.4747768377165027</v>
       </c>
-      <c r="F39" s="95"/>
+      <c r="F39" s="100"/>
       <c r="G39" s="70">
         <f>E7*E39</f>
         <v>8.4747768377165027</v>
@@ -11114,12 +12180,12 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="96"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="96"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="101"/>
     </row>
     <row r="43" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="59" t="s">
@@ -11298,10 +12364,10 @@
       <c r="D51" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="E51" s="93" t="s">
+      <c r="E51" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="93"/>
+      <c r="F51" s="98"/>
       <c r="G51" s="69" t="s">
         <v>99</v>
       </c>
@@ -11328,11 +12394,11 @@
       <c r="D52" s="38">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="E52" s="94">
+      <c r="E52" s="99">
         <f>G48/(B53*E7+C53*F7+D53)</f>
         <v>22.868136580421616</v>
       </c>
-      <c r="F52" s="95"/>
+      <c r="F52" s="100"/>
       <c r="G52" s="70">
         <f>E7*E52</f>
         <v>22.868136580421616</v>
@@ -11370,12 +12436,12 @@
         <f>D52/(B52+C52+D52)</f>
         <v>0.57534246575342463</v>
       </c>
-      <c r="E53" s="96" t="s">
+      <c r="E53" s="101" t="s">
         <v>187</v>
       </c>
-      <c r="F53" s="96"/>
-      <c r="G53" s="96"/>
-      <c r="H53" s="96"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="101"/>
+      <c r="H53" s="101"/>
       <c r="I53" s="46" t="s">
         <v>112</v>
       </c>
@@ -11384,10 +12450,10 @@
       <c r="B54" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="93" t="s">
+      <c r="E54" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="F54" s="93"/>
+      <c r="F54" s="98"/>
       <c r="G54" s="69" t="s">
         <v>101</v>
       </c>
@@ -11396,11 +12462,11 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E55" s="94">
+      <c r="E55" s="99">
         <f>I48/(B53*E7+C53*F7+D53)</f>
         <v>9.9226518189639901</v>
       </c>
-      <c r="F55" s="95"/>
+      <c r="F55" s="100"/>
       <c r="G55" s="70">
         <f>E7*E55</f>
         <v>9.9226518189639901</v>
@@ -11411,12 +12477,12 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E56" s="96" t="s">
+      <c r="E56" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="F56" s="96"/>
-      <c r="G56" s="96"/>
-      <c r="H56" s="96"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="101"/>
+      <c r="H56" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>